<commit_message>
fix: cadenas de valor
</commit_message>
<xml_diff>
--- a/data/toc/toc_ceaf.xlsx
+++ b/data/toc/toc_ceaf.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5420f79c2d515b70/All/PacificoTaskForce/ptfr/data/toc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="459" documentId="8_{04405090-59D7-4F36-89CF-0C27D58B8C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70798DAA-D56A-460C-A952-EFF0092C0905}"/>
+  <xr:revisionPtr revIDLastSave="611" documentId="8_{04405090-59D7-4F36-89CF-0C27D58B8C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73E0A82D-BD51-4885-A98D-40B15E49EA15}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">edges!$A$1:$E$68</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">nodes!$A$1:$E$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">nodes!$A$1:$E$56</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="58">
   <si>
     <t>from</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>shape</t>
-  </si>
-  <si>
-    <t>ellipse</t>
   </si>
   <si>
     <t>level</t>
@@ -115,97 +112,115 @@
     <t>Asistencia</t>
   </si>
   <si>
-    <t>Otorgamiento de subvenciones</t>
-  </si>
-  <si>
-    <t>Otorga subvenciones</t>
-  </si>
-  <si>
     <t>Implementación de las recomendaciones para la gestión de proyectos</t>
   </si>
   <si>
     <t>Implementa recomendaciones</t>
   </si>
   <si>
-    <t>Articulación</t>
-  </si>
-  <si>
     <t>Autonomía en la presentación, gestión y ejecución de proyectos</t>
   </si>
   <si>
     <t>Autonomía</t>
   </si>
   <si>
-    <t>Elaboración planes autónoma</t>
-  </si>
-  <si>
     <t>Sostenibilidad administrativa, operativa y técnica de la organización</t>
   </si>
   <si>
-    <t>Recursos</t>
-  </si>
-  <si>
-    <t>Relacionamiento organizacional???</t>
-  </si>
-  <si>
     <t>Sostenibilidad</t>
   </si>
   <si>
-    <t>Red de colaboración</t>
-  </si>
-  <si>
     <t>Impacto</t>
   </si>
   <si>
-    <t>Mayor porcentaje de ejecución de proyectos por parte de beneficiarios</t>
-  </si>
-  <si>
-    <t>Más ejecución</t>
-  </si>
-  <si>
-    <t>Visibilizar proyectos</t>
-  </si>
-  <si>
-    <t>Construcción informes</t>
-  </si>
-  <si>
-    <t>Entrega informes</t>
-  </si>
-  <si>
-    <t>Visibilizar sus proyectos etnoeducativos y los de otras organizaciones</t>
-  </si>
-  <si>
-    <t>Construcción de informes</t>
-  </si>
-  <si>
-    <t>Entrega de informes bajo parámetros establecidos</t>
-  </si>
-  <si>
-    <t>Mayor gestión de recursos y nuevas fuentes de financiación</t>
-  </si>
-  <si>
-    <t>Mayor cobertura en personas por parte de las instituciones y organizaciones beneficiarias</t>
-  </si>
-  <si>
-    <t>Incorporación en los proyectos educativos institucionales de prácticas etnoeducativas</t>
-  </si>
-  <si>
-    <t>Estrategia de articulación con las organizaciones etnoeducadoras</t>
-  </si>
-  <si>
-    <t>Autogestión en entrega oportuna de información</t>
-  </si>
-  <si>
     <t xml:space="preserve">Los proyectos etnoeducativos  crean condiciones de no discriminación en las comunidades donde se implementan </t>
   </si>
   <si>
     <t>Mayor apropiación de saberes ancestrales en las comunidades educativas</t>
   </si>
   <si>
-    <t>Más instituciones educativas adoptan enfoques etnoeducativos</t>
-  </si>
-  <si>
-    <t>Construcción correcta de informes</t>
+    <t>Adminitrasción de recursos</t>
+  </si>
+  <si>
+    <t>box</t>
+  </si>
+  <si>
+    <t>Recursos humanos</t>
+  </si>
+  <si>
+    <t>Recursos tecnológicos</t>
+  </si>
+  <si>
+    <t>Recursos Financieros</t>
+  </si>
+  <si>
+    <t>Adecuada ejecución</t>
+  </si>
+  <si>
+    <t>Adecuada ejecución de proyectos por parte de Organizaciones Beneficiarias</t>
+  </si>
+  <si>
+    <t>Diseño de estrategias de visibilización de proyectos etnoeducativos</t>
+  </si>
+  <si>
+    <t>Viabilidad de proyectos</t>
+  </si>
+  <si>
+    <t>Efecto intermedio</t>
+  </si>
+  <si>
+    <t>Viabilidad de proyectos de organizaciones beneficiarias (O VISIBILIDAD?)</t>
+  </si>
+  <si>
+    <t>Incorporación en los proyectos educativos institucionales de prácticas etnoeducativas.</t>
+  </si>
+  <si>
+    <t>Proyectos institucionales</t>
+  </si>
+  <si>
+    <t>Diseño e implementación de una red de organizaciones etnoeducadoras.</t>
+  </si>
+  <si>
+    <t>Red de organizaciones etnoeducadoras</t>
+  </si>
+  <si>
+    <t>Mejor gestión de recursos y nuevas fuentes de financiación.</t>
+  </si>
+  <si>
+    <t>Más cobertura en personas por parte de las instituciones y organizaciones beneficiarias</t>
+  </si>
+  <si>
+    <t>Apropiación de red de instituciones etnoeducativas por parte de la comunidad</t>
+  </si>
+  <si>
+    <t>Mejor gestión y nuevas fuentes</t>
+  </si>
+  <si>
+    <t>Más cobertura</t>
+  </si>
+  <si>
+    <t>Condiciones de no discriminación en comunidades</t>
+  </si>
+  <si>
+    <t>Apropiación saberes ancestrales</t>
+  </si>
+  <si>
+    <t>Apropiación de red de instituciones</t>
+  </si>
+  <si>
+    <t>Estrategia visbilización</t>
+  </si>
+  <si>
+    <t>- Dificultades encontradas en la implementación de las estrategias.</t>
+  </si>
+  <si>
+    <t>- Se disenaron estrategias?
+- en qué consisten?</t>
+  </si>
+  <si>
+    <t>- Se han hecho contactos exploratorios para la incorporación en proyectos institucionales?
+- Cuál ha sido el recibimiento?
+- Qué barreras anticipan para alcanzar este objetivo?</t>
   </si>
 </sst>
 </file>
@@ -224,7 +239,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -233,12 +248,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -253,9 +274,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -275,6 +295,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -290,6 +314,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -595,214 +623,305 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="32.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.81640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="33.453125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="4"/>
-    <col min="6" max="8" width="29.36328125" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="2" width="32.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.81640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="33.453125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="3"/>
+    <col min="6" max="8" width="29.36328125" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="5"/>
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="5"/>
+      <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="5"/>
+      <c r="A4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="5"/>
+      <c r="A5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="5"/>
+      <c r="A6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="5"/>
+      <c r="A7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="A8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="A9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="7"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="5"/>
+      <c r="A32" s="4"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" s="7"/>
+      <c r="A43" s="6"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B47" s="5"/>
+      <c r="B47" s="4"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B48" s="5"/>
+      <c r="B48" s="4"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B49" s="5"/>
+      <c r="B49" s="4"/>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B50" s="5"/>
+      <c r="B50" s="4"/>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B51" s="5"/>
+      <c r="B51" s="4"/>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A70" s="7"/>
+      <c r="A70" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E68" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -825,20 +944,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.1796875" customWidth="1"/>
-    <col min="4" max="4" width="48.08984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="48.08984375" style="1" customWidth="1"/>
     <col min="7" max="7" width="32.7265625" customWidth="1"/>
     <col min="8" max="8" width="27.453125" customWidth="1"/>
     <col min="9" max="9" width="25.453125" customWidth="1"/>
@@ -855,180 +974,177 @@
       <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F6">
         <v>2</v>
       </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>37</v>
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
+      <c r="D8" t="s">
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>42</v>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F9">
         <v>3</v>
@@ -1036,137 +1152,256 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
         <v>40</v>
       </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="G13" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11">
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
         <v>28</v>
       </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13">
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="D14" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="D15" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="D16" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D17" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="D18" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="D19" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="D20" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="4:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="D21" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D22" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" s="1"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A55" s="1"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E58" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A1:E56" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>